<commit_message>
fix diageous menu - fix templates
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOUS/Data/on_premise Template.xlsx
+++ b/Projects/DIAGEOUS/Data/on_premise Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -64,7 +64,7 @@
     <t>Menu</t>
   </si>
   <si>
-    <t>1. Main Menu, Menu – Features, 3. Spirits List Menu, 4. Bottle List Menu, 5. After Dinner / Dessert Menu</t>
+    <t>1. Main Menu, 2. Features Menu, 3. Spirits List Menu, 4. Bottle List Menu, 5. After Dinner / Dessert Menu</t>
   </si>
 </sst>
 </file>
@@ -285,15 +285,15 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.8056680161943"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.4453441295547"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
fix diageous menu - fix template weights
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOUS/Data/on_premise Template.xlsx
+++ b/Projects/DIAGEOUS/Data/on_premise Template.xlsx
@@ -284,16 +284,16 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.4453441295547"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="78.0890688259109"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
@@ -382,7 +382,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,7 +402,7 @@
         <v>0.25</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>